<commit_message>
17.09.2020 MC Sales Details:
</commit_message>
<xml_diff>
--- a/2020/September/All Details/16.09.2020/MC Bank Statement Sep-2020.xlsx
+++ b/2020/September/All Details/16.09.2020/MC Bank Statement Sep-2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="August 2020" sheetId="7" r:id="rId1"/>
@@ -2912,18 +2912,54 @@
     <xf numFmtId="2" fontId="39" fillId="35" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="11" fillId="43" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="11" fillId="43" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="11" fillId="43" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="39" fillId="35" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="39" fillId="35" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="39" fillId="35" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="39" fillId="35" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2934,42 +2970,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="11" fillId="43" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="11" fillId="43" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="11" fillId="43" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="39" fillId="35" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="39" fillId="35" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="39" fillId="35" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="39" fillId="35" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3063,7 +3063,7 @@
         <xdr:cNvPr id="1845" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3075,7 +3075,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3098,14 +3098,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3142,7 +3142,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3154,7 +3154,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3177,14 +3177,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4695,8 +4695,8 @@
   </sheetPr>
   <dimension ref="A1:AC222"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -10401,8 +10401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BI246"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C115" sqref="C115"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E112" sqref="E112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -21516,94 +21516,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="23.25">
-      <c r="A1" s="333" t="s">
+      <c r="A1" s="325" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="333"/>
-      <c r="C1" s="333"/>
-      <c r="D1" s="333"/>
-      <c r="E1" s="333"/>
-      <c r="F1" s="333"/>
-      <c r="G1" s="333"/>
-      <c r="H1" s="333"/>
-      <c r="I1" s="333"/>
-      <c r="J1" s="333"/>
-      <c r="K1" s="333"/>
-      <c r="L1" s="333"/>
-      <c r="M1" s="333"/>
-      <c r="N1" s="333"/>
-      <c r="O1" s="333"/>
-      <c r="P1" s="333"/>
-      <c r="Q1" s="333"/>
-      <c r="R1" s="333"/>
-      <c r="S1" s="333"/>
+      <c r="B1" s="325"/>
+      <c r="C1" s="325"/>
+      <c r="D1" s="325"/>
+      <c r="E1" s="325"/>
+      <c r="F1" s="325"/>
+      <c r="G1" s="325"/>
+      <c r="H1" s="325"/>
+      <c r="I1" s="325"/>
+      <c r="J1" s="325"/>
+      <c r="K1" s="325"/>
+      <c r="L1" s="325"/>
+      <c r="M1" s="325"/>
+      <c r="N1" s="325"/>
+      <c r="O1" s="325"/>
+      <c r="P1" s="325"/>
+      <c r="Q1" s="325"/>
+      <c r="R1" s="325"/>
+      <c r="S1" s="325"/>
     </row>
     <row r="2" spans="1:26" s="245" customFormat="1" ht="18">
-      <c r="A2" s="334" t="s">
+      <c r="A2" s="326" t="s">
         <v>161</v>
       </c>
-      <c r="B2" s="334"/>
-      <c r="C2" s="334"/>
-      <c r="D2" s="334"/>
-      <c r="E2" s="334"/>
-      <c r="F2" s="334"/>
-      <c r="G2" s="334"/>
-      <c r="H2" s="334"/>
-      <c r="I2" s="334"/>
-      <c r="J2" s="334"/>
-      <c r="K2" s="334"/>
-      <c r="L2" s="334"/>
-      <c r="M2" s="334"/>
-      <c r="N2" s="334"/>
-      <c r="O2" s="334"/>
-      <c r="P2" s="334"/>
-      <c r="Q2" s="334"/>
-      <c r="R2" s="334"/>
-      <c r="S2" s="334"/>
+      <c r="B2" s="326"/>
+      <c r="C2" s="326"/>
+      <c r="D2" s="326"/>
+      <c r="E2" s="326"/>
+      <c r="F2" s="326"/>
+      <c r="G2" s="326"/>
+      <c r="H2" s="326"/>
+      <c r="I2" s="326"/>
+      <c r="J2" s="326"/>
+      <c r="K2" s="326"/>
+      <c r="L2" s="326"/>
+      <c r="M2" s="326"/>
+      <c r="N2" s="326"/>
+      <c r="O2" s="326"/>
+      <c r="P2" s="326"/>
+      <c r="Q2" s="326"/>
+      <c r="R2" s="326"/>
+      <c r="S2" s="326"/>
     </row>
     <row r="3" spans="1:26" s="245" customFormat="1">
-      <c r="A3" s="335"/>
-      <c r="B3" s="335"/>
-      <c r="C3" s="335"/>
-      <c r="D3" s="335"/>
-      <c r="E3" s="335"/>
-      <c r="F3" s="335"/>
-      <c r="G3" s="335"/>
-      <c r="H3" s="335"/>
-      <c r="I3" s="335"/>
-      <c r="J3" s="335"/>
-      <c r="K3" s="335"/>
-      <c r="L3" s="335"/>
-      <c r="M3" s="335"/>
-      <c r="N3" s="335"/>
-      <c r="O3" s="335"/>
-      <c r="P3" s="335"/>
-      <c r="Q3" s="335"/>
-      <c r="R3" s="335"/>
-      <c r="S3" s="335"/>
+      <c r="A3" s="327"/>
+      <c r="B3" s="327"/>
+      <c r="C3" s="327"/>
+      <c r="D3" s="327"/>
+      <c r="E3" s="327"/>
+      <c r="F3" s="327"/>
+      <c r="G3" s="327"/>
+      <c r="H3" s="327"/>
+      <c r="I3" s="327"/>
+      <c r="J3" s="327"/>
+      <c r="K3" s="327"/>
+      <c r="L3" s="327"/>
+      <c r="M3" s="327"/>
+      <c r="N3" s="327"/>
+      <c r="O3" s="327"/>
+      <c r="P3" s="327"/>
+      <c r="Q3" s="327"/>
+      <c r="R3" s="327"/>
+      <c r="S3" s="327"/>
     </row>
     <row r="4" spans="1:26" s="246" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A4" s="336" t="s">
+      <c r="A4" s="328" t="s">
         <v>162</v>
       </c>
-      <c r="B4" s="337"/>
-      <c r="C4" s="337"/>
-      <c r="D4" s="337"/>
-      <c r="E4" s="337"/>
-      <c r="F4" s="337"/>
-      <c r="G4" s="337"/>
-      <c r="H4" s="337"/>
-      <c r="I4" s="337"/>
-      <c r="J4" s="337"/>
-      <c r="K4" s="337"/>
-      <c r="L4" s="337"/>
-      <c r="M4" s="337"/>
-      <c r="N4" s="337"/>
-      <c r="O4" s="337"/>
-      <c r="P4" s="337"/>
-      <c r="Q4" s="337"/>
-      <c r="R4" s="337"/>
-      <c r="S4" s="338"/>
+      <c r="B4" s="329"/>
+      <c r="C4" s="329"/>
+      <c r="D4" s="329"/>
+      <c r="E4" s="329"/>
+      <c r="F4" s="329"/>
+      <c r="G4" s="329"/>
+      <c r="H4" s="329"/>
+      <c r="I4" s="329"/>
+      <c r="J4" s="329"/>
+      <c r="K4" s="329"/>
+      <c r="L4" s="329"/>
+      <c r="M4" s="329"/>
+      <c r="N4" s="329"/>
+      <c r="O4" s="329"/>
+      <c r="P4" s="329"/>
+      <c r="Q4" s="329"/>
+      <c r="R4" s="329"/>
+      <c r="S4" s="330"/>
       <c r="U4" s="127"/>
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
@@ -21612,58 +21612,58 @@
       <c r="Z4" s="29"/>
     </row>
     <row r="5" spans="1:26" s="248" customFormat="1">
-      <c r="A5" s="339" t="s">
+      <c r="A5" s="331" t="s">
         <v>163</v>
       </c>
-      <c r="B5" s="341" t="s">
+      <c r="B5" s="333" t="s">
         <v>164</v>
       </c>
-      <c r="C5" s="327" t="s">
+      <c r="C5" s="335" t="s">
         <v>165</v>
       </c>
-      <c r="D5" s="327" t="s">
+      <c r="D5" s="335" t="s">
         <v>166</v>
       </c>
-      <c r="E5" s="327" t="s">
+      <c r="E5" s="335" t="s">
         <v>167</v>
       </c>
-      <c r="F5" s="327" t="s">
+      <c r="F5" s="335" t="s">
         <v>168</v>
       </c>
-      <c r="G5" s="327" t="s">
+      <c r="G5" s="335" t="s">
         <v>169</v>
       </c>
-      <c r="H5" s="327" t="s">
+      <c r="H5" s="335" t="s">
         <v>170</v>
       </c>
-      <c r="I5" s="327" t="s">
+      <c r="I5" s="335" t="s">
         <v>171</v>
       </c>
-      <c r="J5" s="327" t="s">
+      <c r="J5" s="335" t="s">
         <v>172</v>
       </c>
-      <c r="K5" s="327" t="s">
+      <c r="K5" s="335" t="s">
         <v>173</v>
       </c>
-      <c r="L5" s="327" t="s">
+      <c r="L5" s="335" t="s">
         <v>174</v>
       </c>
-      <c r="M5" s="327" t="s">
+      <c r="M5" s="335" t="s">
         <v>175</v>
       </c>
-      <c r="N5" s="327" t="s">
+      <c r="N5" s="335" t="s">
         <v>176</v>
       </c>
-      <c r="O5" s="329" t="s">
+      <c r="O5" s="341" t="s">
         <v>177</v>
       </c>
-      <c r="P5" s="331" t="s">
+      <c r="P5" s="343" t="s">
         <v>178</v>
       </c>
-      <c r="Q5" s="325" t="s">
+      <c r="Q5" s="339" t="s">
         <v>31</v>
       </c>
-      <c r="R5" s="343" t="s">
+      <c r="R5" s="337" t="s">
         <v>179</v>
       </c>
       <c r="S5" s="247" t="s">
@@ -21676,24 +21676,24 @@
       <c r="Y5" s="250"/>
     </row>
     <row r="6" spans="1:26" s="248" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A6" s="340"/>
-      <c r="B6" s="342"/>
-      <c r="C6" s="328"/>
-      <c r="D6" s="328"/>
-      <c r="E6" s="328"/>
-      <c r="F6" s="328"/>
-      <c r="G6" s="328"/>
-      <c r="H6" s="328"/>
-      <c r="I6" s="328"/>
-      <c r="J6" s="328"/>
-      <c r="K6" s="328"/>
-      <c r="L6" s="328"/>
-      <c r="M6" s="328"/>
-      <c r="N6" s="328"/>
-      <c r="O6" s="330"/>
-      <c r="P6" s="332"/>
-      <c r="Q6" s="326"/>
-      <c r="R6" s="344"/>
+      <c r="A6" s="332"/>
+      <c r="B6" s="334"/>
+      <c r="C6" s="336"/>
+      <c r="D6" s="336"/>
+      <c r="E6" s="336"/>
+      <c r="F6" s="336"/>
+      <c r="G6" s="336"/>
+      <c r="H6" s="336"/>
+      <c r="I6" s="336"/>
+      <c r="J6" s="336"/>
+      <c r="K6" s="336"/>
+      <c r="L6" s="336"/>
+      <c r="M6" s="336"/>
+      <c r="N6" s="336"/>
+      <c r="O6" s="342"/>
+      <c r="P6" s="344"/>
+      <c r="Q6" s="340"/>
+      <c r="R6" s="338"/>
       <c r="S6" s="252" t="s">
         <v>180</v>
       </c>
@@ -24847,6 +24847,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A3:S3"/>
@@ -24863,12 +24869,6 @@
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="K5:K6"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>